<commit_message>
I added the explanation sheet to explain the data explicitly.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDCE63E-F6AE-204B-A0AE-E9C8E6FC27F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="560" yWindow="500" windowWidth="34360" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Explanation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,18 +21,18 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Yazar</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
@@ -39,37 +41,56 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Number of time periods</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Number of time periods</t>
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Yazar:
-number of commodities</t>
+          <t xml:space="preserve">Yazar:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>number of commodities</t>
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
@@ -78,22 +99,31 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Number of nodes</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Number of nodes</t>
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
@@ -102,206 +132,296 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-First column: Origin Node
-Second Column: Destionation Node</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">First column: Origin Node
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Second Column: Destionation Node</t>
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-B</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>B</t>
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Sikt</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sikt</t>
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-djkt</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>djkt</t>
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Cijkt
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Cijkt
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Uijt</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Uijt</t>
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-blocked</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>blocked</t>
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0">
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-bt</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>bt</t>
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yazar:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-aij</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>aij</t>
         </r>
       </text>
     </comment>
@@ -310,16 +430,232 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Number of time periods</t>
+  </si>
+  <si>
+    <t>Number of commodities</t>
+  </si>
+  <si>
+    <t>Number of nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example: </t>
+  </si>
+  <si>
+    <t>….</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">All possible edges: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Node numbers in A represents the starting point, node numbers in B represents the finishing point of an arc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">B:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Set of blocked arcs: 0 means not blocked, 1 means blocked</t>
+    </r>
+  </si>
+  <si>
+    <t>Example:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">S_ijkt: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Newly arised supply of commodity k at node i in period t</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">dijkt: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Newly arised demand of commodity k at node i in period t</t>
+    </r>
+  </si>
+  <si>
+    <t>8 (node 1 is a supply node in this time period)</t>
+  </si>
+  <si>
+    <t>0 (node 1 has 0 demand in this period)</t>
+  </si>
+  <si>
+    <t>1 (arc 14 is blocked in time period t)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cijkt: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Unit travel time on arc (i,j) for commodity k time period t</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Uijt: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Capacity of arc (i,j) in time period t</t>
+    </r>
+  </si>
+  <si>
+    <t>Column2: Arc (i,j) information of commodity 2 - time period 1</t>
+  </si>
+  <si>
+    <t>Column1: Arc (i,j) information of commodity 1 - time period 1</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>Column k: Arc (i,j) information of commodity k - time period 1</t>
+  </si>
+  <si>
+    <t>Column k*t: Arc (i,j) information of commodity k - time period t</t>
+  </si>
+  <si>
+    <t>4 column for a variable means 2 commodity - 2 time period.</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">blocked: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Optional information on the blockness situation of the arc in time period t</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (0 if blocked, 1 if not. We multiply this with the capacity to get the adjusted capacities)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bt: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Units of road restoration resources in time period t</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aij: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Number of resources needed to restore the blocked arc in time period t</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,20 +664,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +741,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -397,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -405,6 +780,59 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,19 +1112,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView topLeftCell="J1" zoomScale="141" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="18" max="19" width="8.88671875" customWidth="1"/>
+    <col min="18" max="19" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -764,7 +1192,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -832,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -900,7 +1328,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -964,7 +1392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1028,7 +1456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1092,7 +1520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1156,7 +1584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1220,7 +1648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -1284,7 +1712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1348,7 +1776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -1412,7 +1840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1476,7 +1904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -1540,7 +1968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -1604,7 +2032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1668,7 +2096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -1732,7 +2160,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -1796,7 +2224,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>3</v>
       </c>
@@ -1860,7 +2288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>3</v>
       </c>
@@ -1924,7 +2352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -1988,7 +2416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -2052,7 +2480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -2116,7 +2544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -2180,7 +2608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -2244,7 +2672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>4</v>
       </c>
@@ -2308,7 +2736,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>4</v>
       </c>
@@ -2372,7 +2800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>5</v>
       </c>
@@ -2436,7 +2864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>5</v>
       </c>
@@ -2500,7 +2928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>5</v>
       </c>
@@ -2564,7 +2992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>5</v>
       </c>
@@ -2628,7 +3056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>5</v>
       </c>
@@ -2692,7 +3120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>5</v>
       </c>
@@ -2756,7 +3184,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>6</v>
       </c>
@@ -2820,7 +3248,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>6</v>
       </c>
@@ -2884,7 +3312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>6</v>
       </c>
@@ -2948,7 +3376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>6</v>
       </c>
@@ -3012,7 +3440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>6</v>
       </c>
@@ -3076,7 +3504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>6</v>
       </c>
@@ -3144,4 +3572,907 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E9574B-418C-C44F-BC8C-2BB678B15129}">
+  <dimension ref="A2:V30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="137" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.33203125" customWidth="1"/>
+    <col min="21" max="21" width="24" customWidth="1"/>
+    <col min="22" max="22" width="29.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="21"/>
+      <c r="T3" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="27"/>
+      <c r="V3" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="5"/>
+      <c r="T4" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="U4" s="3"/>
+      <c r="V4" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="13">
+        <v>0</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="8">
+        <v>1</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="26">
+        <v>12</v>
+      </c>
+      <c r="U5" s="26"/>
+      <c r="V5" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="17">
+        <v>8</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="9">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="13">
+        <v>10</v>
+      </c>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="17">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="8">
+        <v>1</v>
+      </c>
+      <c r="S6" s="5"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0</v>
+      </c>
+      <c r="D7" s="17">
+        <v>8</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="13">
+        <v>8</v>
+      </c>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="17">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="8">
+        <v>1</v>
+      </c>
+      <c r="S7" s="5"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="17">
+        <v>8</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="13">
+        <v>2</v>
+      </c>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="17">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="5"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8">
+        <v>5</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0</v>
+      </c>
+      <c r="D9" s="17">
+        <v>8</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="13">
+        <v>2</v>
+      </c>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="17">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="8">
+        <v>1</v>
+      </c>
+      <c r="S9" s="5"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8">
+        <v>6</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0</v>
+      </c>
+      <c r="D10" s="17">
+        <v>8</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="13">
+        <v>1</v>
+      </c>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="17">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="8">
+        <v>1</v>
+      </c>
+      <c r="S10" s="5"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" s="5"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="2"/>
+    </row>
+    <row r="18" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="2"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="2"/>
+    </row>
+    <row r="20" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="2"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="2"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="2"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="2"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="2"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="2"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="2"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="2"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="2"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="2"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:O3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Constraint 4 changed (install openpyxl to read excel)
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDCE63E-F6AE-204B-A0AE-E9C8E6FC27F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745D7F95-D896-0143-AB3A-9A3040674F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="34360" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="500" windowWidth="34360" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -803,35 +803,35 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1115,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="141" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1271,16 +1271,16 @@
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E3" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H3" s="5">
         <v>0</v>
@@ -1339,16 +1339,16 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H4" s="5">
         <v>0</v>
@@ -1403,16 +1403,16 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H5" s="5">
         <v>0</v>
@@ -1467,16 +1467,16 @@
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E6" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H6" s="5">
         <v>0</v>
@@ -1531,16 +1531,16 @@
         <v>0</v>
       </c>
       <c r="D7" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E7" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F7" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H7" s="5">
         <v>0</v>
@@ -1595,16 +1595,16 @@
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E8" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H8" s="5">
         <v>0</v>
@@ -1659,16 +1659,16 @@
         <v>0</v>
       </c>
       <c r="D9" s="3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E9" s="3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F9" s="3">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G9" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H9" s="5">
         <v>0</v>
@@ -1723,16 +1723,16 @@
         <v>0</v>
       </c>
       <c r="D10" s="3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E10" s="3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F10" s="3">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G10" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H10" s="5">
         <v>0</v>
@@ -1787,16 +1787,16 @@
         <v>1</v>
       </c>
       <c r="D11" s="3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F11" s="3">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G11" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H11" s="5">
         <v>0</v>
@@ -1851,16 +1851,16 @@
         <v>0</v>
       </c>
       <c r="D12" s="3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F12" s="3">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G12" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H12" s="5">
         <v>0</v>
@@ -1915,16 +1915,16 @@
         <v>0</v>
       </c>
       <c r="D13" s="3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E13" s="3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F13" s="3">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G13" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H13" s="5">
         <v>0</v>
@@ -1979,16 +1979,16 @@
         <v>0</v>
       </c>
       <c r="D14" s="3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E14" s="3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F14" s="3">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G14" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>0</v>
@@ -3578,7 +3578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E9574B-418C-C44F-BC8C-2BB678B15129}">
   <dimension ref="A2:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="137" workbookViewId="0">
+    <sheetView zoomScale="137" workbookViewId="0">
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
@@ -3597,55 +3597,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="A2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="21" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="23" t="s">
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="18" t="s">
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="21" t="s">
+      <c r="Q3" s="25"/>
+      <c r="R3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="21"/>
+      <c r="S3" s="26"/>
       <c r="T3" s="27" t="s">
         <v>26</v>
       </c>
       <c r="U3" s="27"/>
-      <c r="V3" s="29" t="s">
+      <c r="V3" s="24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3683,11 +3683,11 @@
         <v>9</v>
       </c>
       <c r="S4" s="5"/>
-      <c r="T4" s="24" t="s">
+      <c r="T4" s="20" t="s">
         <v>9</v>
       </c>
       <c r="U4" s="3"/>
-      <c r="V4" s="25" t="s">
+      <c r="V4" s="21" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3727,11 +3727,11 @@
         <v>1</v>
       </c>
       <c r="S5" s="5"/>
-      <c r="T5" s="26">
+      <c r="T5" s="22">
         <v>12</v>
       </c>
-      <c r="U5" s="26"/>
-      <c r="V5" s="28">
+      <c r="U5" s="22"/>
+      <c r="V5" s="23">
         <v>8</v>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       <c r="S6" s="5"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
-      <c r="V6" s="28">
+      <c r="V6" s="23">
         <v>8</v>
       </c>
     </row>
@@ -3815,7 +3815,7 @@
       <c r="S7" s="5"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
-      <c r="V7" s="28">
+      <c r="V7" s="23">
         <v>8</v>
       </c>
     </row>
@@ -3857,7 +3857,7 @@
       <c r="S8" s="5"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
-      <c r="V8" s="28">
+      <c r="V8" s="23">
         <v>8</v>
       </c>
     </row>
@@ -3899,7 +3899,7 @@
       <c r="S9" s="5"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
-      <c r="V9" s="28">
+      <c r="V9" s="23">
         <v>8</v>
       </c>
     </row>
@@ -3941,7 +3941,7 @@
       <c r="S10" s="5"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
-      <c r="V10" s="28">
+      <c r="V10" s="23">
         <v>8</v>
       </c>
     </row>
@@ -3983,7 +3983,7 @@
       <c r="S11" s="5"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
-      <c r="V11" s="28" t="s">
+      <c r="V11" s="23" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4044,7 +4044,7 @@
     <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="14"/>

</xml_diff>

<commit_message>
supply < demand data.xlsx changed for loop for all objectives
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745D7F95-D896-0143-AB3A-9A3040674F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD673D6-5632-9740-B677-763FCFCED028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="500" windowWidth="34360" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1116,7 +1116,7 @@
   <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1271,13 +1271,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F3" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -1339,13 +1339,13 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E4" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F4" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G4" s="3">
         <v>2</v>
@@ -1403,13 +1403,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G5" s="3">
         <v>2</v>
@@ -1467,13 +1467,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E6" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G6" s="3">
         <v>2</v>
@@ -1531,13 +1531,13 @@
         <v>0</v>
       </c>
       <c r="D7" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F7" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G7" s="3">
         <v>2</v>
@@ -1595,13 +1595,13 @@
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F8" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G8" s="3">
         <v>2</v>
@@ -1665,7 +1665,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -1729,7 +1729,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
@@ -1793,7 +1793,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G11" s="3">
         <v>1</v>
@@ -1857,7 +1857,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G12" s="3">
         <v>1</v>
@@ -1921,7 +1921,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G13" s="3">
         <v>1</v>
@@ -1985,7 +1985,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G14" s="3">
         <v>1</v>

</xml_diff>

<commit_message>
output excel creator loop fixed
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD673D6-5632-9740-B677-763FCFCED028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC55A41-2AC7-F943-85EA-8895B74935FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="500" windowWidth="34360" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1116,7 +1116,7 @@
   <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2055,16 +2055,16 @@
         <v>0</v>
       </c>
       <c r="H15" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I15" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J15" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K15" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L15" s="4">
         <v>1</v>
@@ -2119,16 +2119,16 @@
         <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I16" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J16" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K16" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L16" s="4">
         <v>2</v>
@@ -2183,16 +2183,16 @@
         <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I17" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J17" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K17" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L17" s="4">
         <v>0</v>
@@ -2247,16 +2247,16 @@
         <v>0</v>
       </c>
       <c r="H18" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I18" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J18" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K18" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L18" s="4">
         <v>3</v>
@@ -2311,16 +2311,16 @@
         <v>0</v>
       </c>
       <c r="H19" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I19" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J19" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K19" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L19" s="4">
         <v>2</v>
@@ -2375,16 +2375,16 @@
         <v>0</v>
       </c>
       <c r="H20" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I20" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J20" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K20" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L20" s="4">
         <v>2</v>
@@ -2439,16 +2439,16 @@
         <v>0</v>
       </c>
       <c r="H21" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I21" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J21" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K21" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L21" s="4">
         <v>3</v>
@@ -2503,16 +2503,16 @@
         <v>0</v>
       </c>
       <c r="H22" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I22" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J22" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K22" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L22" s="4">
         <v>1</v>
@@ -2567,16 +2567,16 @@
         <v>0</v>
       </c>
       <c r="H23" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I23" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J23" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K23" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L23" s="4">
         <v>1</v>
@@ -2631,16 +2631,16 @@
         <v>0</v>
       </c>
       <c r="H24" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I24" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J24" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K24" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L24" s="4">
         <v>0</v>
@@ -2695,16 +2695,16 @@
         <v>0</v>
       </c>
       <c r="H25" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I25" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J25" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K25" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L25" s="4">
         <v>2</v>
@@ -2759,16 +2759,16 @@
         <v>0</v>
       </c>
       <c r="H26" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I26" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J26" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K26" s="5">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L26" s="4">
         <v>2</v>

</xml_diff>